<commit_message>
parse new profession category
</commit_message>
<xml_diff>
--- a/Professions/41 Юриспруденция.xlsx
+++ b/Professions/41 Юриспруденция.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="320">
   <si>
     <t>ID</t>
   </si>
@@ -197,16 +197,121 @@
     <t>Описание</t>
   </si>
   <si>
-    <t>это специалист, который помогает мирно разрешать конфликты, а также предупреждать их возникновение</t>
+    <t>Конфликтолог-это специалист, который помогает мирно разрешать конфликты, а также предупреждать их возникновение</t>
   </si>
   <si>
-    <t>это специалист, призванный содействовать разрешению конфликтов между людьми, организациями и сообществами посредством проведения процедуры медиации.</t>
+    <t>Медиатор-это специалист, призванный содействовать разрешению конфликтов между людьми, организациями и сообществами посредством проведения процедуры медиации.</t>
   </si>
   <si>
-    <t>это специалист, обладающий багажом знаний, необходимых для всестороннего изучения имеющихся документов, пожеланий сторон, и составления на их основе соответствующего договора</t>
+    <t>Договорной юрист-это специалист, обладающий багажом знаний, необходимых для всестороннего изучения имеющихся документов, пожеланий сторон, и составления на их основе соответствующего договора</t>
   </si>
   <si>
-    <t>это специалист, ведущий деятельность, сосредоточенную на выдвижении и отстаивании законных и юридически обоснованных требований об исполнении обязательств контрагентами организации-работодателя</t>
+    <t>Специалист претензионного отдела-это специалист, ведущий деятельность, сосредоточенную на выдвижении и отстаивании законных и юридически обоснованных требований об исполнении обязательств контрагентами организации-работодателя</t>
+  </si>
+  <si>
+    <t>Юрист по правовой экспертизе контрактов-это специалист, который проверяет контракты на соотвествие законодательной базе</t>
+  </si>
+  <si>
+    <t>Юрист судебник – человек, отстаивающий в судах первой, апелляционной, кассационной инстанций интересы предприятий, граждан.</t>
+  </si>
+  <si>
+    <t>Юрист по гражданскому праву-это специалист в области гражданского права. Сама по себе отрасль гражданского права чрезвычайно обширна и потому гражданский юрист это специалист достаточно широкого профиля. Гражданский юрист может иметь свою специализацию в области договорного права, жилищного права, семейного права и так далее.</t>
+  </si>
+  <si>
+    <t>Юрист арбитражник- лицо, оказывающее юридические услуги по сопровождению коммерческой деятельности компаний.</t>
+  </si>
+  <si>
+    <t>Юрист по трудовому праву – это специалист, который не только знает как действовать при разрешении трудового спора, но и способен избежать проблем во взаимоотношениях работника с работодателем, не доводя конфликт до судебного разбирательства.</t>
+  </si>
+  <si>
+    <t>Юрист по уголовному праву-специалист в области уголовного права, имеющий полномочия защитника в уголовном процессе, наделенный процессуальными правами и обязанностями в рамках уголовного дела.</t>
+  </si>
+  <si>
+    <t>Юрист по административным делам осуществляет детальный анализ правонарушения с точки зрения права, подготавливает документы для подачи заявления в суд и принимает активное участие в судебном разбирательстве.</t>
+  </si>
+  <si>
+    <t>Юрист по конституционному праву - это правовой специалист защищающий интересы клиентов на основе Конституции, являющейся основным законом и содержащей нормы прямого действия.</t>
+  </si>
+  <si>
+    <t>Юрист по интеллектуальному праву – высококвалифицированный специалист в области права, имеющий узкую специализацию в направлении юридического сопровождения и защиты нематериальной собственности.</t>
+  </si>
+  <si>
+    <t>Сетевой юрист – специалист, в задачу которого входит формирование нормативно-правового взаимодействия в Сети, в том числе, в виртуальных мирах.</t>
+  </si>
+  <si>
+    <t>Юрист по морскому праву (морской юрист) сопровождают транграничные морские проекты, лежащие в различных юрисдикциях, и специализируется на международном морском частном праве. Это подотрасль международного частного права, которая регулирует имущественные отношения, осложнённые иностранным элементом, возникающие в процессе международного экономического оборота и связанные с морепользованием.</t>
+  </si>
+  <si>
+    <t>Юрист-международник — это специалист по международному праву. Как правило, он занимается юридическим обеспечением сделок между различными национальными компаниями.</t>
+  </si>
+  <si>
+    <t>Адвокат — лицо, профессией которого является оказание квалифицированной юридической помощи физическим лицам (гражданам, лицам без гражданства) и юридическим лицам (организациям), в том числе защита их прав и представление интересов в суде, обладающее полученным в установленном порядке статусом адвоката.</t>
+  </si>
+  <si>
+    <t>Адвокат по гражданскому праву-это юрист, специализацией которого является ведение гражданских дел различного профиля. Адвокаты по гражданским делам отстаивают в суде интересы истцов, ответчиков.</t>
+  </si>
+  <si>
+    <t>Адвокат по арбитражу поможет не только грамотно составить исковое заявление, но и приложит к нему все нужные документы, выстроит содержательную часть с учетом всех тонкостей арбитражного процесса.</t>
+  </si>
+  <si>
+    <t>Адвокат по трудовому праву-это специалист, который не только знает как действовать при разрешении трудового спора, но и способен избежать проблем во взаимоотношениях работника с работодателем, не доводя конфликт до судебного разбирательства.</t>
+  </si>
+  <si>
+    <t>Адвокат по уголовному праву - независимый профессиональный советник, обладающий правом осуществлять адвокатскую деятельность. Советник оказывает консультационные, представительские услуги участникам (сторонам) дела: подозреваемым в совершении общественно-опасного деяния.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Адвокат по административному праву специализируется на предоставлении помощи, касающейся решения различных проблем в сферах, регулируемых административным законодательством. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Адвокат по конституционному праву— лицо, профессией которого является оказание квалифицированной юридической помощи физическим лицам (гражданам, лицам без гражданства) и юридическим лицам (организациям) по конституционному праву</t>
+  </si>
+  <si>
+    <t>Адвокат по интеллектуальному праву— лицо, профессией которого является оказание квалифицированной юридической помощи физическим лицам (гражданам, лицам без гражданства) и юридическим лицам  (организациям) по интеллектуальному праву.</t>
+  </si>
+  <si>
+    <t>Юриско́нсульт — правовед, штатный работник организации (юридического лица), обеспечивающий соблюдение законодательства, как организацией, так и по отношению к организации со стороны иных участников правоотношений.</t>
+  </si>
+  <si>
+    <t>Виртуальный адвокат - специалист, который обеспечивает своему клиенту юридическую поддержку через Интернет с использованием различных онлайн коммуникаторов.</t>
+  </si>
+  <si>
+    <t>Судья — должностное лицо, входящее в состав суда и осуществляющее правосудие; в современной теории разделения властей — лицо, наделённое судебной властью.</t>
+  </si>
+  <si>
+    <t>Мировой судья — лицо, наделённое полномочиями выполнять функции мировых судов. Мировые суды представляют собой местные юридические органы низшей инстанции, обладающие ограниченной юрисдикцией и рассматривающие малозначительные дела по упрощённой процедуре.</t>
+  </si>
+  <si>
+    <t>Районный судья-это судья,осуществляет судебные полномочия на уровне субъекта.</t>
+  </si>
+  <si>
+    <t>Конституционне судьи -судьи судебного органа, самостоятельно осуществляющего посредством конституционного судопроизводства конституционный контроль.</t>
+  </si>
+  <si>
+    <t>Верховный судья- это судья по гражданским делам, делам по разрешению экономических споров, уголовным, административным и иным делам. Осуществляет в предусмотренных федеральным законом процессуальных формах судебный надзор за деятельностью судов, рассматривая гражданские дела, дела по разрешению экономических споров, уголовные, административные и иные дела, в качестве суда надзорной инстанции, а также в пределах своей компетенции в качестве суда апелляционной и кассационной инстанций.</t>
+  </si>
+  <si>
+    <t>Арбитражный судья– это судья, осуществляющий правосудие в сфере предпринимательства и иной экономической деятельности путем разрешения экономических споров и рассмотрения иных дел, отнесенных к его компетенции.</t>
+  </si>
+  <si>
+    <t>Судьями военных судов являются лица, наделенные в конституционном порядке полномочиями осуществлять правосудие и исполняющие свои обязанности на профессиональной основе в Вооруженных Силах Российской Федерации.</t>
+  </si>
+  <si>
+    <t>Специалист по судебному администрированию– это профессионал, который разбирается во всех тонкостях судопроизводства и создаёт условия для осуществления правосудия в РФ.</t>
+  </si>
+  <si>
+    <t>Секретарь суда – это специалист, который работает с документами, делает ксерокопии и подшивки документов, работает с оргтехникой, ведет протоколы судебных заседаний, а также осуществляет набор информации на компьютере.</t>
+  </si>
+  <si>
+    <t>Судебные приставы — это государственные служащие, которые следят за безопасностью и соблюдением порядка в судах, исполняют вступившие в силу судебные акты и контролируют работу коллекторских агентств.</t>
+  </si>
+  <si>
+    <t>Судебный эксперт – специалист, выполняющий экспертизу, результаты которой в последствии используются во время судебного процесса. Заключение эксперта помогает суду принять взвешенное и объективное решение.</t>
+  </si>
+  <si>
+    <t>Нотариус-лицо, специально уполномоченное на совершение нотариальных действий, среди которых свидетельствование верности копий документов и выписок из них, свидетельствование подлинности подписи на документах, свидетельствование верности перевода документов с одного языка на другой, а также некоторые другие действия, нормы которых отличаются друг от друга в различных странах.</t>
+  </si>
+  <si>
+    <t>Патентовед – специалист по оформлению заявок на регистрацию изобретений.</t>
   </si>
   <si>
     <t>Функции 1</t>
@@ -346,6 +451,117 @@
   </si>
   <si>
     <t>https://ka-lex.ru/wp-content/uploads/2016/05/1829187801_6.jpg</t>
+  </si>
+  <si>
+    <t>https://s1.stc.all.kpcdn.net/putevoditel/projectid_346574/images/tild6636-6538-4237-b337-646539666530__shutterstock_1061449.jpg</t>
+  </si>
+  <si>
+    <t>https://amperasound.ru/upload/iblock/1d2/1d28380d2883956f8ec2826422f6b58d.jpeg</t>
+  </si>
+  <si>
+    <t>https://advacademy.ru/images/orator-v-syde.jpg</t>
+  </si>
+  <si>
+    <t>https://avatars.mds.yandex.net/get-zen_doc/1917783/pub_609ff856774aa53d3182f44e_609ff87276444c347510e088/scale_1200</t>
+  </si>
+  <si>
+    <t>https://aquachainik.ru/wp-content/uploads/2021/08/2341.jpg</t>
+  </si>
+  <si>
+    <t>https://avatars.mds.yandex.net/get-altay/1773749/2a0000016a4df4f81e603531537840de10f6/XXL</t>
+  </si>
+  <si>
+    <t>https://avatars.mds.yandex.net/get-altay/2004078/2a000001767b5d328bd887933f493f30f9b1/XXXL</t>
+  </si>
+  <si>
+    <t>https://egevpare.ru/wp-content/uploads/2022/03/6481_4.jpg</t>
+  </si>
+  <si>
+    <t>https://storage.yandexcloud.net/vyksavkurse-files/1/ueLuZTCa6eBDEFoXQlrSPX-JrSZX409v.jpg</t>
+  </si>
+  <si>
+    <t>http://www.yurist-troitsk.ru/wp-content/uploads/2019/12/yurist-Moskva.jpg</t>
+  </si>
+  <si>
+    <t>https://ffb.ranepa.ru/images/mobile-worke214124124r-1.jpg</t>
+  </si>
+  <si>
+    <t>https://cdn2.postupi.online/images/images335x232/28/099.jpg</t>
+  </si>
+  <si>
+    <t>https://bankstoday.net/wp-content/uploads/2020/09/right-4944546_1920.jpg</t>
+  </si>
+  <si>
+    <t>https://dirksen-lawyer.ru/wp-content/uploads/2017/08/Investment-management-lawyers-benefit-from-regulatory-burden-.jpg</t>
+  </si>
+  <si>
+    <t>https://tsoka.ru/wp-content/uploads/2022/03/istock-975593000-scaled-1.jpg</t>
+  </si>
+  <si>
+    <t>http://wums.ru/wp-content/uploads/2021/05/sa2.jpg</t>
+  </si>
+  <si>
+    <t>https://avatars.mds.yandex.net/get-zen_doc/1581919/pub_5e5e34dbf848ee31c81803dd_5e5e35c407fa2c0a6634aefb/scale_1200</t>
+  </si>
+  <si>
+    <t>https://lawyer-nikolaev.ru/wp-content/uploads/2017/08/Lawyer-Selection.jpg</t>
+  </si>
+  <si>
+    <t>https://psb-advoco.ru/assets/images/background-05.jpg</t>
+  </si>
+  <si>
+    <t>https://ecologicaonline.ru/img/86b045860c82969d28f1adffb2b6fc51.jpg</t>
+  </si>
+  <si>
+    <t>https://fitcapital.ru/img/574896.jpg</t>
+  </si>
+  <si>
+    <t>https://www.stangerlaw.com/wp-content/uploads/2019/02/What-You-Need-for-a-Product-Liability-Lawsuit.jpg</t>
+  </si>
+  <si>
+    <t>https://fb.ru/media/i/1/9/1/2/4/0/4/i/1912404.jpg</t>
+  </si>
+  <si>
+    <t>https://img.p-advice.com/img/entertainment/847/9-reasons-to-settle-instead-of-go-to-divorce-court_7.jpg</t>
+  </si>
+  <si>
+    <t>https://static.mk.ru/upload/objects/photoreportsImages/detailPicture/28/49/bf/ad/2252326_6292363.jpg</t>
+  </si>
+  <si>
+    <t>https://serovglobus.ru/upload/iblock/ff3/ff3e3196dd4c240c48007826a64fa17d.jpg</t>
+  </si>
+  <si>
+    <t>https://static.360tv.ru/media/images/articles/cover/c59476b8-3cd9-46d7-a6fb-d73c3055a134/57566765.jpg</t>
+  </si>
+  <si>
+    <t>https://oc-media.org/app/uploads/2019/12/russian-supreme-court.jpg</t>
+  </si>
+  <si>
+    <t>https://avatars.mds.yandex.net/get-zen_doc/5235248/pub_60ed3a892cf7e07073b1c35b_60ed3c3aa0fd024896a93865/scale_1200</t>
+  </si>
+  <si>
+    <t>http://files.sudrf.ru/628/press_dep/Gal30img516e82cd323aa.jpg</t>
+  </si>
+  <si>
+    <t>http://files.sudrf.ru/2374/user/DSCN0005.jpg</t>
+  </si>
+  <si>
+    <t>https://komi.arbitr.ru/files/images/3_0.JPG</t>
+  </si>
+  <si>
+    <t>https://nsk.bfm.ru/storage/article/June2021/3aTPk5stS7BxpDjug8Px4RkLAMAkXmzvv5pLkaX4.jpg</t>
+  </si>
+  <si>
+    <t>http://proforientir42.ru/wp-content/uploads/2021/10/sud.jpg</t>
+  </si>
+  <si>
+    <t>http://remontmechty.ru/wp-content/uploads/2021/07/%D0%AD%D0%BA%D1%81%D0%BF%D0%B5%D1%80%D1%82%D0%B8%D0%B7%D0%B0-%D0%BF%D0%BE-%D1%84%D0%B0%D0%BA%D1%82%D1%83-%D1%81%D0%BC%D0%B5%D1%80%D1%82%D0%B8-1522228254.jpg</t>
+  </si>
+  <si>
+    <t>https://narcosis-css.ru/800/600/https/trainingplaces.ca/static/img/career/logo/Law_Clerk.jpg</t>
+  </si>
+  <si>
+    <t>https://voronezh.skidkom.ru/static/content/35279/common/biznes-i-finansy/35279_15937665967660.jpg</t>
   </si>
   <si>
     <t>Навык 1</t>
@@ -775,7 +991,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -806,6 +1022,10 @@
     <font>
       <sz val="10.0"/>
       <color rgb="FF202124"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -882,7 +1102,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,6 +1113,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEA9999"/>
+        <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
     <fill>
@@ -911,7 +1137,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -961,26 +1187,36 @@
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
@@ -988,64 +1224,67 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -7966,32 +8205,32 @@
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>177</v>
+      <c r="C1" s="38" t="s">
+        <v>249</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>178</v>
+        <v>250</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>179</v>
+        <v>251</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="33" t="s">
-        <v>180</v>
+      <c r="G1" s="38" t="s">
+        <v>252</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>181</v>
+        <v>253</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>182</v>
+        <v>254</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>183</v>
+        <v>255</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>184</v>
+        <v>256</v>
       </c>
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
@@ -12196,20 +12435,20 @@
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>185</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>186</v>
-      </c>
-      <c r="F1" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="G1" s="34" t="s">
-        <v>188</v>
+      <c r="C1" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>259</v>
+      </c>
+      <c r="G1" s="39" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="2">
@@ -12219,11 +12458,11 @@
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3">
       <c r="A3" s="4">
@@ -12232,11 +12471,11 @@
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
     </row>
     <row r="4">
       <c r="A4" s="4">
@@ -12245,11 +12484,11 @@
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
     </row>
     <row r="5">
       <c r="A5" s="4">
@@ -12258,11 +12497,11 @@
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="44"/>
     </row>
     <row r="6">
       <c r="A6" s="4">
@@ -12271,11 +12510,11 @@
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
     </row>
     <row r="7">
       <c r="A7" s="4">
@@ -12284,11 +12523,11 @@
       <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="36"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="41"/>
     </row>
     <row r="8">
       <c r="A8" s="4">
@@ -12297,11 +12536,11 @@
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="38"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="43"/>
     </row>
     <row r="9">
       <c r="A9" s="4">
@@ -12310,11 +12549,11 @@
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
     </row>
     <row r="10">
       <c r="A10" s="4">
@@ -12323,11 +12562,11 @@
       <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
     </row>
     <row r="11">
       <c r="A11" s="4">
@@ -12344,11 +12583,11 @@
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
     </row>
     <row r="13">
       <c r="A13" s="4">
@@ -12357,11 +12596,11 @@
       <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="14">
       <c r="A14" s="4">
@@ -12370,11 +12609,11 @@
       <c r="B14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
     </row>
     <row r="15">
       <c r="A15" s="4">
@@ -12383,11 +12622,11 @@
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
     </row>
     <row r="16">
       <c r="A16" s="4">
@@ -12396,11 +12635,11 @@
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="36"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="41"/>
     </row>
     <row r="17">
       <c r="A17" s="4">
@@ -12409,11 +12648,11 @@
       <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
     </row>
     <row r="18">
       <c r="A18" s="4">
@@ -12422,11 +12661,11 @@
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
     </row>
     <row r="19">
       <c r="A19" s="4">
@@ -12435,11 +12674,11 @@
       <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="20">
       <c r="A20" s="4">
@@ -12448,11 +12687,11 @@
       <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
     </row>
     <row r="21">
       <c r="A21" s="4">
@@ -12461,11 +12700,11 @@
       <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="43"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="48"/>
     </row>
     <row r="22">
       <c r="A22" s="4">
@@ -12506,7 +12745,7 @@
       <c r="B26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="25"/>
+      <c r="F26" s="30"/>
     </row>
     <row r="27">
       <c r="A27" s="4">
@@ -12531,7 +12770,7 @@
       <c r="B29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F29" s="25"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30">
       <c r="A30" s="4">
@@ -12540,7 +12779,7 @@
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="25"/>
+      <c r="C30" s="30"/>
     </row>
     <row r="31">
       <c r="A31" s="4">
@@ -12885,11 +13124,11 @@
     <row r="104">
       <c r="A104" s="4"/>
       <c r="B104" s="7"/>
-      <c r="C104" s="36"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
-      <c r="F104" s="36"/>
-      <c r="G104" s="36"/>
+      <c r="C104" s="41"/>
+      <c r="D104" s="41"/>
+      <c r="E104" s="41"/>
+      <c r="F104" s="41"/>
+      <c r="G104" s="41"/>
     </row>
     <row r="105">
       <c r="A105" s="4"/>
@@ -12930,10 +13169,10 @@
     <row r="114">
       <c r="A114" s="4"/>
       <c r="B114" s="7"/>
-      <c r="D114" s="36"/>
-      <c r="E114" s="36"/>
-      <c r="F114" s="36"/>
-      <c r="G114" s="36"/>
+      <c r="D114" s="41"/>
+      <c r="E114" s="41"/>
+      <c r="F114" s="41"/>
+      <c r="G114" s="41"/>
     </row>
     <row r="115">
       <c r="A115" s="4"/>
@@ -13053,9 +13292,9 @@
     <row r="144">
       <c r="A144" s="4"/>
       <c r="B144" s="7"/>
-      <c r="E144" s="30"/>
-      <c r="F144" s="37"/>
-      <c r="G144" s="43"/>
+      <c r="E144" s="35"/>
+      <c r="F144" s="42"/>
+      <c r="G144" s="48"/>
     </row>
     <row r="145">
       <c r="A145" s="4"/>
@@ -13280,11 +13519,11 @@
     <row r="200">
       <c r="A200" s="4"/>
       <c r="B200" s="7"/>
-      <c r="C200" s="36"/>
-      <c r="D200" s="36"/>
-      <c r="E200" s="36"/>
-      <c r="F200" s="36"/>
-      <c r="G200" s="36"/>
+      <c r="C200" s="41"/>
+      <c r="D200" s="41"/>
+      <c r="E200" s="41"/>
+      <c r="F200" s="41"/>
+      <c r="G200" s="41"/>
     </row>
     <row r="201">
       <c r="A201" s="4"/>
@@ -13293,11 +13532,11 @@
     <row r="202">
       <c r="A202" s="4"/>
       <c r="B202" s="7"/>
-      <c r="C202" s="36"/>
-      <c r="D202" s="36"/>
-      <c r="E202" s="36"/>
-      <c r="F202" s="36"/>
-      <c r="G202" s="36"/>
+      <c r="C202" s="41"/>
+      <c r="D202" s="41"/>
+      <c r="E202" s="41"/>
+      <c r="F202" s="41"/>
+      <c r="G202" s="41"/>
     </row>
     <row r="203">
       <c r="A203" s="4"/>
@@ -13306,10 +13545,10 @@
     <row r="204">
       <c r="A204" s="4"/>
       <c r="B204" s="7"/>
-      <c r="D204" s="36"/>
-      <c r="E204" s="36"/>
-      <c r="F204" s="36"/>
-      <c r="G204" s="36"/>
+      <c r="D204" s="41"/>
+      <c r="E204" s="41"/>
+      <c r="F204" s="41"/>
+      <c r="G204" s="41"/>
     </row>
     <row r="205">
       <c r="A205" s="4"/>
@@ -13322,20 +13561,20 @@
     <row r="207">
       <c r="A207" s="4"/>
       <c r="B207" s="7"/>
-      <c r="C207" s="42"/>
-      <c r="D207" s="36"/>
-      <c r="E207" s="36"/>
-      <c r="F207" s="36"/>
-      <c r="G207" s="36"/>
+      <c r="C207" s="47"/>
+      <c r="D207" s="41"/>
+      <c r="E207" s="41"/>
+      <c r="F207" s="41"/>
+      <c r="G207" s="41"/>
     </row>
     <row r="208">
       <c r="A208" s="4"/>
       <c r="B208" s="7"/>
-      <c r="C208" s="36"/>
-      <c r="D208" s="36"/>
-      <c r="E208" s="36"/>
-      <c r="F208" s="42"/>
-      <c r="G208" s="36"/>
+      <c r="C208" s="41"/>
+      <c r="D208" s="41"/>
+      <c r="E208" s="41"/>
+      <c r="F208" s="47"/>
+      <c r="G208" s="41"/>
     </row>
     <row r="209">
       <c r="A209" s="4"/>
@@ -13359,7 +13598,7 @@
     <row r="214">
       <c r="A214" s="4"/>
       <c r="B214" s="7"/>
-      <c r="C214" s="25"/>
+      <c r="C214" s="30"/>
     </row>
     <row r="215">
       <c r="A215" s="4"/>
@@ -13476,34 +13715,34 @@
     <row r="243">
       <c r="A243" s="4"/>
       <c r="B243" s="7"/>
-      <c r="C243" s="44"/>
+      <c r="C243" s="49"/>
     </row>
     <row r="244">
       <c r="A244" s="4"/>
-      <c r="B244" s="36"/>
-      <c r="C244" s="36"/>
-      <c r="D244" s="36"/>
-      <c r="E244" s="36"/>
-      <c r="F244" s="40"/>
-      <c r="G244" s="36"/>
+      <c r="B244" s="41"/>
+      <c r="C244" s="41"/>
+      <c r="D244" s="41"/>
+      <c r="E244" s="41"/>
+      <c r="F244" s="45"/>
+      <c r="G244" s="41"/>
     </row>
     <row r="245">
       <c r="A245" s="4"/>
       <c r="B245" s="7"/>
-      <c r="C245" s="36"/>
-      <c r="D245" s="36"/>
-      <c r="E245" s="36"/>
-      <c r="F245" s="36"/>
-      <c r="G245" s="36"/>
+      <c r="C245" s="41"/>
+      <c r="D245" s="41"/>
+      <c r="E245" s="41"/>
+      <c r="F245" s="41"/>
+      <c r="G245" s="41"/>
     </row>
     <row r="246">
       <c r="A246" s="4"/>
       <c r="B246" s="7"/>
-      <c r="C246" s="36"/>
-      <c r="D246" s="36"/>
-      <c r="E246" s="36"/>
-      <c r="F246" s="36"/>
-      <c r="G246" s="36"/>
+      <c r="C246" s="41"/>
+      <c r="D246" s="41"/>
+      <c r="E246" s="41"/>
+      <c r="F246" s="41"/>
+      <c r="G246" s="41"/>
     </row>
     <row r="247">
       <c r="A247" s="4"/>
@@ -13684,12 +13923,12 @@
     <row r="291">
       <c r="A291" s="4"/>
       <c r="B291" s="7"/>
-      <c r="C291" s="37"/>
-      <c r="D291" s="30"/>
-      <c r="E291" s="32"/>
-      <c r="F291" s="30"/>
-      <c r="G291" s="43"/>
-      <c r="H291" s="30"/>
+      <c r="C291" s="42"/>
+      <c r="D291" s="35"/>
+      <c r="E291" s="37"/>
+      <c r="F291" s="35"/>
+      <c r="G291" s="48"/>
+      <c r="H291" s="35"/>
     </row>
     <row r="292">
       <c r="A292" s="4"/>
@@ -16560,17 +16799,17 @@
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="33" t="s">
-        <v>189</v>
+      <c r="C1" s="38" t="s">
+        <v>261</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>190</v>
+        <v>262</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>188</v>
+        <v>258</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>260</v>
       </c>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
@@ -16599,14 +16838,14 @@
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>193</v>
+      <c r="C2" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="3">
@@ -16616,14 +16855,14 @@
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>196</v>
+      <c r="C3" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="4">
@@ -16633,14 +16872,14 @@
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>199</v>
+      <c r="C4" s="29" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="5">
@@ -16650,9 +16889,9 @@
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="41"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="46"/>
     </row>
     <row r="6">
       <c r="A6" s="4">
@@ -16757,9 +16996,9 @@
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="37"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="42"/>
     </row>
     <row r="19">
       <c r="A19" s="4">
@@ -17451,8 +17690,8 @@
     <row r="167">
       <c r="A167" s="4"/>
       <c r="B167" s="7"/>
-      <c r="D167" s="30"/>
-      <c r="E167" s="30"/>
+      <c r="D167" s="35"/>
+      <c r="E167" s="35"/>
     </row>
     <row r="168">
       <c r="A168" s="4"/>
@@ -20817,77 +21056,77 @@
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>212</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>214</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>216</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="Y1" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>223</v>
+      <c r="C1" s="23" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>282</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>284</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>287</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>288</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>293</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="2">
@@ -22022,7 +22261,7 @@
     </row>
     <row r="244">
       <c r="A244" s="4"/>
-      <c r="B244" s="36"/>
+      <c r="B244" s="41"/>
     </row>
     <row r="245">
       <c r="A245" s="4"/>
@@ -25074,77 +25313,77 @@
       <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="G1" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>232</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>238</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>239</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>240</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="Y1" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>247</v>
+      <c r="C1" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>299</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>303</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>304</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>306</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>307</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>308</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>311</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>312</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>313</v>
+      </c>
+      <c r="U1" s="23" t="s">
+        <v>314</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="2">
@@ -26279,7 +26518,7 @@
     </row>
     <row r="244">
       <c r="A244" s="4"/>
-      <c r="B244" s="36"/>
+      <c r="B244" s="41"/>
     </row>
     <row r="245">
       <c r="A245" s="4"/>
@@ -34475,7 +34714,9 @@
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4">
@@ -34484,7 +34725,9 @@
       <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="4">
@@ -34493,7 +34736,9 @@
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="4">
@@ -34502,7 +34747,9 @@
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4">
@@ -34511,7 +34758,9 @@
       <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4">
@@ -34520,7 +34769,9 @@
       <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4">
@@ -34529,7 +34780,9 @@
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4">
@@ -34538,16 +34791,43 @@
       <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="4">
+      <c r="A14" s="17">
         <v>13.0</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
     </row>
     <row r="15">
       <c r="A15" s="4">
@@ -34556,7 +34836,9 @@
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4">
@@ -34565,7 +34847,9 @@
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="4">
@@ -34574,7 +34858,9 @@
       <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="4">
@@ -34583,7 +34869,9 @@
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="C18" s="7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="4">
@@ -34592,7 +34880,9 @@
       <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4">
@@ -34601,7 +34891,9 @@
       <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="4">
@@ -34610,7 +34902,9 @@
       <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="4">
@@ -34619,7 +34913,9 @@
       <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="4">
@@ -34628,7 +34924,9 @@
       <c r="B23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="7"/>
+      <c r="C23" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="4">
@@ -34637,7 +34935,9 @@
       <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="7"/>
+      <c r="C24" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="4">
@@ -34646,7 +34946,9 @@
       <c r="B25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="7"/>
+      <c r="C25" s="21" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="4">
@@ -34655,7 +34957,9 @@
       <c r="B26" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="7"/>
+      <c r="C26" s="7" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="4">
@@ -34664,7 +34968,9 @@
       <c r="B27" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="4">
@@ -34673,7 +34979,9 @@
       <c r="B28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="4">
@@ -34682,7 +34990,9 @@
       <c r="B29" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="7"/>
+      <c r="C29" s="7" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="4">
@@ -34691,7 +35001,9 @@
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="7"/>
+      <c r="C30" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="4">
@@ -34700,7 +35012,9 @@
       <c r="B31" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="7"/>
+      <c r="C31" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="4">
@@ -34709,7 +35023,9 @@
       <c r="B32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="7"/>
+      <c r="C32" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="4">
@@ -34718,7 +35034,9 @@
       <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="7"/>
+      <c r="C33" s="7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="4">
@@ -34727,16 +35045,43 @@
       <c r="B34" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="4">
+      <c r="A35" s="17">
         <v>34.0</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="7"/>
+      <c r="C35" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+      <c r="S35" s="20"/>
+      <c r="T35" s="20"/>
+      <c r="U35" s="20"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="20"/>
+      <c r="X35" s="20"/>
+      <c r="Y35" s="20"/>
+      <c r="Z35" s="20"/>
     </row>
     <row r="36">
       <c r="A36" s="4">
@@ -34745,7 +35090,9 @@
       <c r="B36" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="7"/>
+      <c r="C36" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="4">
@@ -34754,16 +35101,43 @@
       <c r="B37" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="4">
+      <c r="A38" s="17">
         <v>37.0</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="20"/>
+      <c r="S38" s="20"/>
+      <c r="T38" s="20"/>
+      <c r="U38" s="20"/>
+      <c r="V38" s="20"/>
+      <c r="W38" s="20"/>
+      <c r="X38" s="20"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
     </row>
     <row r="39">
       <c r="A39" s="4">
@@ -34772,7 +35146,9 @@
       <c r="B39" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="4">
@@ -34781,7 +35157,9 @@
       <c r="B40" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="4">
@@ -34790,16 +35168,43 @@
       <c r="B41" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="7" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="4">
+      <c r="A42" s="17">
         <v>41.0</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="20"/>
     </row>
     <row r="43">
       <c r="A43" s="4"/>
@@ -39620,61 +40025,61 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>62</v>
+        <v>97</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>63</v>
+        <v>98</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>66</v>
+        <v>101</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>76</v>
+        <v>111</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="V1" s="11"/>
       <c r="W1" s="11"/>
@@ -39687,23 +40092,23 @@
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>85</v>
+      <c r="C2" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3">
@@ -39713,23 +40118,23 @@
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>91</v>
+      <c r="C3" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4">
@@ -39739,26 +40144,26 @@
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>98</v>
+      <c r="C4" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="5">
@@ -39768,17 +40173,17 @@
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>102</v>
+      <c r="C5" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="6">
@@ -42600,7 +43005,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -42633,8 +43038,8 @@
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>104</v>
+      <c r="C2" s="28" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="3">
@@ -42644,8 +43049,8 @@
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>105</v>
+      <c r="C3" s="29" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="4">
@@ -42655,8 +43060,8 @@
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>106</v>
+      <c r="C4" s="29" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5">
@@ -42666,7 +43071,9 @@
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="25"/>
+      <c r="C5" s="28" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="4">
@@ -42675,6 +43082,9 @@
       <c r="B6" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="C6" s="29" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="4">
@@ -42683,6 +43093,9 @@
       <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="C7" s="29" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="4">
@@ -42691,6 +43104,9 @@
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="29" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="4">
@@ -42699,6 +43115,9 @@
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="29" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="4">
@@ -42707,6 +43126,9 @@
       <c r="B10" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="C10" s="29" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="4">
@@ -42715,6 +43137,9 @@
       <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="C11" s="29" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4">
@@ -42723,6 +43148,9 @@
       <c r="B12" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="C12" s="29" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="4">
@@ -42731,6 +43159,9 @@
       <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
+      <c r="C13" s="29" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4">
@@ -42739,6 +43170,9 @@
       <c r="B14" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="C14" s="29" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="4">
@@ -42747,6 +43181,9 @@
       <c r="B15" s="6" t="s">
         <v>22</v>
       </c>
+      <c r="C15" s="29" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4">
@@ -42755,6 +43192,9 @@
       <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="C16" s="29" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="4">
@@ -42763,6 +43203,9 @@
       <c r="B17" s="6" t="s">
         <v>24</v>
       </c>
+      <c r="C17" s="29" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="4">
@@ -42771,7 +43214,9 @@
       <c r="B18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="25"/>
+      <c r="C18" s="28" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="4">
@@ -42780,7 +43225,9 @@
       <c r="B19" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="25"/>
+      <c r="C19" s="28" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="4">
@@ -42789,7 +43236,9 @@
       <c r="B20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="25"/>
+      <c r="C20" s="28" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="4">
@@ -42798,7 +43247,9 @@
       <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="25"/>
+      <c r="C21" s="28" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="4">
@@ -42807,6 +43258,9 @@
       <c r="B22" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="C22" s="29" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="4">
@@ -42815,6 +43269,9 @@
       <c r="B23" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="C23" s="29" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="4">
@@ -42823,6 +43280,9 @@
       <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="C24" s="29" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="4">
@@ -42831,6 +43291,9 @@
       <c r="B25" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="C25" s="29" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="4">
@@ -42839,6 +43302,9 @@
       <c r="B26" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="C26" s="29" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="4">
@@ -42847,6 +43313,9 @@
       <c r="B27" s="6" t="s">
         <v>34</v>
       </c>
+      <c r="C27" s="29" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="4">
@@ -42855,6 +43324,9 @@
       <c r="B28" s="6" t="s">
         <v>36</v>
       </c>
+      <c r="C28" s="29" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="4">
@@ -42863,6 +43335,9 @@
       <c r="B29" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="C29" s="29" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="4">
@@ -42871,6 +43346,9 @@
       <c r="B30" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="C30" s="29" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="4">
@@ -42879,7 +43357,9 @@
       <c r="B31" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="25"/>
+      <c r="C31" s="28" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="4">
@@ -42888,6 +43368,9 @@
       <c r="B32" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="C32" s="29" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="4">
@@ -42896,6 +43379,9 @@
       <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
+      <c r="C33" s="29" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="4">
@@ -42904,6 +43390,9 @@
       <c r="B34" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="C34" s="29" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="4">
@@ -42912,6 +43401,9 @@
       <c r="B35" s="6" t="s">
         <v>43</v>
       </c>
+      <c r="C35" s="29" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="4">
@@ -42920,6 +43412,9 @@
       <c r="B36" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="C36" s="29" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="4">
@@ -42928,6 +43423,9 @@
       <c r="B37" s="6" t="s">
         <v>45</v>
       </c>
+      <c r="C37" s="29" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="4">
@@ -42936,6 +43434,9 @@
       <c r="B38" s="6" t="s">
         <v>43</v>
       </c>
+      <c r="C38" s="29" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="4">
@@ -42944,6 +43445,9 @@
       <c r="B39" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="C39" s="29" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="4">
@@ -42952,6 +43456,9 @@
       <c r="B40" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="C40" s="29" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="4">
@@ -42960,7 +43467,9 @@
       <c r="B41" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="25"/>
+      <c r="C41" s="28" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="4">
@@ -42969,6 +43478,9 @@
       <c r="B42" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="C42" s="29" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="4"/>
@@ -42989,7 +43501,7 @@
     <row r="47">
       <c r="A47" s="4"/>
       <c r="B47" s="7"/>
-      <c r="C47" s="25"/>
+      <c r="C47" s="30"/>
     </row>
     <row r="48">
       <c r="A48" s="4"/>
@@ -43006,7 +43518,7 @@
     <row r="51">
       <c r="A51" s="4"/>
       <c r="B51" s="7"/>
-      <c r="C51" s="25"/>
+      <c r="C51" s="30"/>
     </row>
     <row r="52">
       <c r="A52" s="4"/>
@@ -43111,7 +43623,7 @@
     <row r="77">
       <c r="A77" s="4"/>
       <c r="B77" s="7"/>
-      <c r="C77" s="25"/>
+      <c r="C77" s="30"/>
     </row>
     <row r="78">
       <c r="A78" s="4"/>
@@ -43220,7 +43732,7 @@
     <row r="104">
       <c r="A104" s="4"/>
       <c r="B104" s="7"/>
-      <c r="C104" s="25"/>
+      <c r="C104" s="30"/>
     </row>
     <row r="105">
       <c r="A105" s="4"/>
@@ -43237,7 +43749,7 @@
     <row r="108">
       <c r="A108" s="4"/>
       <c r="B108" s="7"/>
-      <c r="C108" s="25"/>
+      <c r="C108" s="30"/>
     </row>
     <row r="109">
       <c r="A109" s="4"/>
@@ -43258,7 +43770,7 @@
     <row r="113">
       <c r="A113" s="4"/>
       <c r="B113" s="7"/>
-      <c r="C113" s="25"/>
+      <c r="C113" s="30"/>
     </row>
     <row r="114">
       <c r="A114" s="4"/>
@@ -43295,7 +43807,7 @@
     <row r="122">
       <c r="A122" s="4"/>
       <c r="B122" s="7"/>
-      <c r="C122" s="25"/>
+      <c r="C122" s="30"/>
     </row>
     <row r="123">
       <c r="A123" s="4"/>
@@ -43515,7 +44027,7 @@
     <row r="177">
       <c r="A177" s="4"/>
       <c r="B177" s="7"/>
-      <c r="C177" s="25"/>
+      <c r="C177" s="30"/>
     </row>
     <row r="178">
       <c r="A178" s="4"/>
@@ -43556,7 +44068,7 @@
     <row r="187">
       <c r="A187" s="4"/>
       <c r="B187" s="7"/>
-      <c r="C187" s="25"/>
+      <c r="C187" s="30"/>
     </row>
     <row r="188">
       <c r="A188" s="4"/>
@@ -43664,7 +44176,7 @@
     <row r="214">
       <c r="A214" s="4"/>
       <c r="B214" s="7"/>
-      <c r="C214" s="25"/>
+      <c r="C214" s="30"/>
     </row>
     <row r="215">
       <c r="A215" s="4"/>
@@ -43813,7 +44325,7 @@
     <row r="251">
       <c r="A251" s="4"/>
       <c r="B251" s="7"/>
-      <c r="C251" s="25"/>
+      <c r="C251" s="30"/>
     </row>
     <row r="252">
       <c r="A252" s="4"/>
@@ -43838,7 +44350,7 @@
     <row r="257">
       <c r="A257" s="4"/>
       <c r="B257" s="7"/>
-      <c r="C257" s="25"/>
+      <c r="C257" s="30"/>
     </row>
     <row r="258">
       <c r="A258" s="4"/>
@@ -43899,7 +44411,7 @@
     <row r="272">
       <c r="A272" s="4"/>
       <c r="B272" s="7"/>
-      <c r="C272" s="25"/>
+      <c r="C272" s="30"/>
     </row>
     <row r="273">
       <c r="A273" s="4"/>
@@ -43924,7 +44436,7 @@
     <row r="278">
       <c r="A278" s="4"/>
       <c r="B278" s="7"/>
-      <c r="C278" s="25"/>
+      <c r="C278" s="30"/>
     </row>
     <row r="279">
       <c r="A279" s="4"/>
@@ -43949,7 +44461,7 @@
     <row r="284">
       <c r="A284" s="4"/>
       <c r="B284" s="7"/>
-      <c r="C284" s="25"/>
+      <c r="C284" s="30"/>
     </row>
     <row r="285">
       <c r="A285" s="4"/>
@@ -44074,7 +44586,7 @@
     <row r="315">
       <c r="A315" s="4"/>
       <c r="B315" s="6"/>
-      <c r="C315" s="25"/>
+      <c r="C315" s="30"/>
     </row>
     <row r="316">
       <c r="A316" s="4"/>
@@ -46822,8 +47334,46 @@
     <hyperlink r:id="rId1" ref="C2"/>
     <hyperlink r:id="rId2" ref="C3"/>
     <hyperlink r:id="rId3" ref="C4"/>
+    <hyperlink r:id="rId4" ref="C5"/>
+    <hyperlink r:id="rId5" ref="C6"/>
+    <hyperlink r:id="rId6" ref="C7"/>
+    <hyperlink r:id="rId7" ref="C8"/>
+    <hyperlink r:id="rId8" ref="C9"/>
+    <hyperlink r:id="rId9" ref="C10"/>
+    <hyperlink r:id="rId10" ref="C11"/>
+    <hyperlink r:id="rId11" ref="C12"/>
+    <hyperlink r:id="rId12" ref="C13"/>
+    <hyperlink r:id="rId13" ref="C14"/>
+    <hyperlink r:id="rId14" ref="C15"/>
+    <hyperlink r:id="rId15" ref="C16"/>
+    <hyperlink r:id="rId16" ref="C17"/>
+    <hyperlink r:id="rId17" ref="C18"/>
+    <hyperlink r:id="rId18" ref="C19"/>
+    <hyperlink r:id="rId19" ref="C20"/>
+    <hyperlink r:id="rId20" ref="C21"/>
+    <hyperlink r:id="rId21" ref="C22"/>
+    <hyperlink r:id="rId22" ref="C23"/>
+    <hyperlink r:id="rId23" ref="C24"/>
+    <hyperlink r:id="rId24" ref="C25"/>
+    <hyperlink r:id="rId25" ref="C26"/>
+    <hyperlink r:id="rId26" ref="C27"/>
+    <hyperlink r:id="rId27" ref="C28"/>
+    <hyperlink r:id="rId28" ref="C29"/>
+    <hyperlink r:id="rId29" ref="C30"/>
+    <hyperlink r:id="rId30" ref="C31"/>
+    <hyperlink r:id="rId31" ref="C32"/>
+    <hyperlink r:id="rId32" ref="C33"/>
+    <hyperlink r:id="rId33" ref="C34"/>
+    <hyperlink r:id="rId34" ref="C35"/>
+    <hyperlink r:id="rId35" ref="C36"/>
+    <hyperlink r:id="rId36" ref="C37"/>
+    <hyperlink r:id="rId37" ref="C38"/>
+    <hyperlink r:id="rId38" ref="C39"/>
+    <hyperlink r:id="rId39" ref="C40"/>
+    <hyperlink r:id="rId40" ref="C41"/>
+    <hyperlink r:id="rId41" ref="C42"/>
   </hyperlinks>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId42"/>
 </worksheet>
 </file>
 
@@ -46852,64 +47402,64 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>108</v>
+        <v>180</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>109</v>
+        <v>181</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>110</v>
+        <v>182</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>111</v>
+        <v>183</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>112</v>
+        <v>184</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>113</v>
+        <v>185</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>115</v>
+        <v>187</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>116</v>
+        <v>188</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>117</v>
+        <v>189</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>118</v>
+        <v>190</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>119</v>
+        <v>191</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>120</v>
+        <v>192</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>121</v>
+        <v>193</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>122</v>
+        <v>194</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>123</v>
+        <v>195</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>124</v>
+        <v>196</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>125</v>
+        <v>197</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>126</v>
+        <v>198</v>
       </c>
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
@@ -46923,20 +47473,20 @@
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>131</v>
+      <c r="C2" s="31" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="3">
@@ -46946,26 +47496,26 @@
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>137</v>
+      <c r="C3" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="4">
@@ -46975,20 +47525,20 @@
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>131</v>
+      <c r="C4" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="5">
@@ -46998,8 +47548,8 @@
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="E5" s="28"/>
+      <c r="C5" s="32"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6">
       <c r="A6" s="4">
@@ -47024,9 +47574,9 @@
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="9">
       <c r="A9" s="4">
@@ -47131,10 +47681,10 @@
       <c r="B21" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22">
       <c r="A22" s="4">
@@ -49811,7 +50361,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>142</v>
+        <v>214</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="11"/>
@@ -49844,8 +50394,8 @@
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="24" t="s">
-        <v>143</v>
+      <c r="C2" s="29" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="3">
@@ -49855,8 +50405,8 @@
       <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="24" t="s">
-        <v>144</v>
+      <c r="C3" s="29" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="4">
@@ -49866,8 +50416,8 @@
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="24" t="s">
-        <v>145</v>
+      <c r="C4" s="29" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="5">
@@ -54040,76 +54590,76 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>146</v>
+        <v>218</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>147</v>
+        <v>219</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>148</v>
+        <v>220</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>149</v>
+        <v>221</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>150</v>
+        <v>222</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>151</v>
+        <v>223</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>152</v>
+        <v>224</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>153</v>
+        <v>225</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>154</v>
+        <v>226</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>155</v>
+        <v>227</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>156</v>
+        <v>228</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>157</v>
+        <v>229</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>158</v>
+        <v>230</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>159</v>
+        <v>231</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>160</v>
+        <v>232</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>161</v>
+        <v>233</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>162</v>
+        <v>234</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>163</v>
+        <v>235</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>164</v>
+        <v>236</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>165</v>
+        <v>237</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>166</v>
+        <v>238</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>167</v>
+        <v>239</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>168</v>
+        <v>240</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>169</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2">
@@ -54135,11 +54685,11 @@
       <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>171</v>
+      <c r="C4" s="23" t="s">
+        <v>242</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="5">
@@ -58299,41 +58849,41 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>103</v>
+      <c r="A1" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="18" t="s">
-        <v>170</v>
+      <c r="A2" s="23" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="18" t="s">
-        <v>171</v>
+      <c r="A3" s="23" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="18" t="s">
-        <v>173</v>
+      <c r="A4" s="23" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="18" t="s">
-        <v>174</v>
+      <c r="A5" s="23" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="18" t="s">
-        <v>175</v>
+      <c r="A6" s="23" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="18" t="s">
-        <v>176</v>
+      <c r="A7" s="23" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>